<commit_message>
DID A BUNCH OF ODD THINGS but eventually set working directory and rendered up to the end of problem 1
</commit_message>
<xml_diff>
--- a/data/sleep_log.xlsx
+++ b/data/sleep_log.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyattdunn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyattdunn/Desktop/Git/ENVS-193DS_homework-03/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E0C98F4-BC57-EB48-B168-27B0F509721D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFC0CE75-91C8-5845-9BFB-49F2ACDDDB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{4105ABD6-3EEF-444D-9076-E3C2C17AF6C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="realistic_sleep_log_final" sheetId="1" r:id="rId1"/>
+    <sheet name="sleep_log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>